<commit_message>
/ ‘Extended Campuses/Self Appraisals/2015/Data for 2015 year (Better).xlsx’
</commit_message>
<xml_diff>
--- a/Extended Campuses/Self Appraisals/2015/Data for 2015 year (Better).xlsx
+++ b/Extended Campuses/Self Appraisals/2015/Data for 2015 year (Better).xlsx
@@ -15,7 +15,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$B$1:$B$412</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$412</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -1801,7 +1801,7 @@
   <dimension ref="A1:G412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11292,7 +11292,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="B1:B412"/>
+  <autoFilter ref="A1:G412"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>